<commit_message>
Upadate yesterday aтв today actual time
</commit_message>
<xml_diff>
--- a/03.12-14.12.xlsx
+++ b/03.12-14.12.xlsx
@@ -74,6 +74,30 @@
           </rPr>
           <t xml:space="preserve">
 с учетом вычета на английский</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anna Sharuntsova.EXT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+не пошла на английский</t>
         </r>
       </text>
     </comment>
@@ -216,19 +240,19 @@
     <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -519,7 +543,7 @@
   <dimension ref="B2:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:M12"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,32 +577,32 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="9">
         <v>6.75</v>
       </c>
       <c r="E3" s="1">
         <v>0.5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="9">
         <v>7</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="9">
         <v>3.25</v>
       </c>
       <c r="K3" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="9">
         <v>3</v>
       </c>
       <c r="M3" s="6">
@@ -586,53 +610,53 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="9"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="6"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>6.75</v>
       </c>
       <c r="E6" s="1">
         <v>0.51041666666666663</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>7</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <v>5</v>
       </c>
       <c r="K6" s="1">
         <v>0.64583333333333337</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="5">
         <v>4.25</v>
       </c>
       <c r="M6" s="6">
@@ -640,24 +664,24 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="1">
         <v>0.80208333333333337</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="1">
         <v>0.875</v>
       </c>
-      <c r="J7" s="7"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L7" s="7"/>
+      <c r="L7" s="5"/>
       <c r="M7" s="6"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -686,37 +710,37 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>0.5625</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="9">
         <v>4.75</v>
       </c>
       <c r="E11" s="1">
         <v>0.5625</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="9">
         <v>6</v>
       </c>
       <c r="G11" s="1">
         <v>0.6875</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="9">
         <v>2</v>
       </c>
       <c r="I11" s="1">
         <v>0.375</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="9">
         <v>4</v>
       </c>
       <c r="K11" s="1">
         <v>0.6875</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="9">
         <v>3.25</v>
       </c>
       <c r="M11" s="6">
@@ -724,71 +748,99 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="1">
         <v>0.8125</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="6"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="1">
         <v>0.5625</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>4.75</v>
       </c>
       <c r="E14" s="1">
         <v>0.5625</v>
       </c>
-      <c r="F14" s="7">
-        <v>6</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="7"/>
+      <c r="F14" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="H14" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J14" s="5">
+        <v>3</v>
+      </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="7"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="1">
-        <v>0.8125</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="7"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J15" s="5"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="7"/>
+      <c r="L15" s="5"/>
       <c r="M15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="B3:B4"/>
@@ -803,20 +855,6 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update today hours. Again
</commit_message>
<xml_diff>
--- a/03.12-14.12.xlsx
+++ b/03.12-14.12.xlsx
@@ -247,13 +247,11 @@
     <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
@@ -262,7 +260,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
@@ -591,29 +591,29 @@
       <c r="C3" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="10">
         <v>6.75</v>
       </c>
       <c r="E3" s="1">
         <v>0.5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="10">
         <v>7</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="10">
         <v>3.25</v>
       </c>
       <c r="K3" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="10">
         <v>3</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="7">
         <v>20</v>
       </c>
     </row>
@@ -622,24 +622,24 @@
       <c r="C4" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
@@ -651,28 +651,28 @@
       <c r="E6" s="1">
         <v>0.51041666666666663</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>7</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>5</v>
       </c>
       <c r="K6" s="1">
         <v>0.64583333333333337</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>4.25</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
@@ -680,17 +680,17 @@
       <c r="E7" s="1">
         <v>0.80208333333333337</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="1">
         <v>0.875</v>
       </c>
-      <c r="J7" s="7"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -724,34 +724,34 @@
       <c r="C11" s="1">
         <v>0.5625</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="10">
         <v>4.75</v>
       </c>
       <c r="E11" s="1">
         <v>0.5625</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="10">
         <v>6</v>
       </c>
       <c r="G11" s="1">
         <v>0.6875</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="10">
         <v>2</v>
       </c>
       <c r="I11" s="1">
         <v>0.375</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="10">
         <v>4</v>
       </c>
       <c r="K11" s="1">
         <v>0.6875</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="10">
         <v>3.25</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="7">
         <v>20</v>
       </c>
     </row>
@@ -760,89 +760,103 @@
       <c r="C12" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="1">
         <v>0.8125</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="10"/>
       <c r="K12" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="1">
         <v>0.5625</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>4.75</v>
       </c>
       <c r="E14" s="1">
         <v>0.5625</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>5.5</v>
       </c>
       <c r="G14" s="1">
         <v>0.67708333333333337</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>3.5</v>
       </c>
       <c r="I14" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <v>3</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="5">
         <v>0.64583333333333337</v>
       </c>
-      <c r="L14" s="7">
-        <v>4.25</v>
-      </c>
-      <c r="M14" s="6">
-        <v>21</v>
+      <c r="L14" s="6">
+        <v>3.25</v>
+      </c>
+      <c r="M14" s="7">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="6"/>
       <c r="K15" s="1">
-        <v>0.82291666666666663</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="6"/>
+        <v>0.78125</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="B3:B4"/>
@@ -857,20 +871,6 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>